<commit_message>
Mid missions API Contract frontend migration
</commit_message>
<xml_diff>
--- a/Rumi/MschemaBS.xlsx
+++ b/Rumi/MschemaBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4D650A-5BC9-4329-B896-A327020CCFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1432E479-17EE-460A-828E-906A26C925C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CE3A5E2-9228-41D5-BA51-51DDF36D6524}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="330">
   <si>
     <t>clients</t>
   </si>
@@ -990,6 +990,51 @@
   </si>
   <si>
     <t>### Pattern 9: Sensitive Data Encryption (Payment Account Security)</t>
+  </si>
+  <si>
+    <t>### Flow 2: Automatic Creator Onboarding</t>
+  </si>
+  <si>
+    <t>Check after signup API Contract is created</t>
+  </si>
+  <si>
+    <t>Areas of Impact</t>
+  </si>
+  <si>
+    <t>auth pages flow</t>
+  </si>
+  <si>
+    <t>Codex Audit - Architecture musts</t>
+  </si>
+  <si>
+    <t>How creators join program. Two Paths: Cruva-Sourced Creators + Word-of-outh Creators</t>
+  </si>
+  <si>
+    <t>### Flow 3: Creator First-Time Registration</t>
+  </si>
+  <si>
+    <t>### Flow 4: Returning User Login</t>
+  </si>
+  <si>
+    <t>### Flow 5: Password Reset (Magic Link)</t>
+  </si>
+  <si>
+    <t>### Flow 6: Email Verification System (OTP)</t>
+  </si>
+  <si>
+    <t>### Flow 7: Daily Tier Calculation (Automated)</t>
+  </si>
+  <si>
+    <t>Creator Flows</t>
+  </si>
+  <si>
+    <t>### Flow 7: Admin Adds Creator Manually</t>
+  </si>
+  <si>
+    <t>### Flow 8: Creator Claims Reward</t>
+  </si>
+  <si>
+    <t>This is a daily flow, automated. Not related to creators login flows</t>
   </si>
 </sst>
 </file>
@@ -1485,10 +1530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C646EFC9-76BE-47C4-938D-0A30980E5B72}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,9 +1543,10 @@
     <col min="2" max="2" width="47.85546875" customWidth="1"/>
     <col min="3" max="3" width="69.140625" customWidth="1"/>
     <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>278</v>
       </c>
@@ -1512,8 +1559,11 @@
       <c r="D1" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -1521,7 +1571,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -1529,7 +1579,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>279</v>
       </c>
@@ -1537,7 +1587,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>279</v>
       </c>
@@ -1545,7 +1595,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>279</v>
       </c>
@@ -1553,7 +1603,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>279</v>
       </c>
@@ -1561,7 +1611,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>287</v>
       </c>
@@ -1572,7 +1622,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>291</v>
       </c>
@@ -1580,7 +1630,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -1591,7 +1641,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -1599,7 +1649,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>291</v>
       </c>
@@ -1607,7 +1657,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>291</v>
       </c>
@@ -1615,7 +1665,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>291</v>
       </c>
@@ -1623,7 +1673,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -1634,7 +1684,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>298</v>
       </c>
@@ -1642,7 +1692,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>302</v>
       </c>
@@ -1650,7 +1700,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>298</v>
       </c>
@@ -1658,76 +1708,217 @@
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>305</v>
       </c>
       <c r="B19" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>305</v>
       </c>
       <c r="B20" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>305</v>
       </c>
       <c r="B21" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>305</v>
       </c>
       <c r="B22" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>305</v>
       </c>
       <c r="B23" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>305</v>
       </c>
       <c r="B24" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>305</v>
       </c>
       <c r="B25" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>305</v>
       </c>
       <c r="B26" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>305</v>
       </c>
       <c r="B27" t="s">
         <v>314</v>
+      </c>
+      <c r="C27" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>305</v>
+      </c>
+      <c r="B28" t="s">
+        <v>315</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>305</v>
+      </c>
+      <c r="B30" t="s">
+        <v>321</v>
+      </c>
+      <c r="C30" t="s">
+        <v>326</v>
+      </c>
+      <c r="E30" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>305</v>
+      </c>
+      <c r="B31" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" t="s">
+        <v>326</v>
+      </c>
+      <c r="E31" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>305</v>
+      </c>
+      <c r="B32" t="s">
+        <v>323</v>
+      </c>
+      <c r="C32" t="s">
+        <v>326</v>
+      </c>
+      <c r="E32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B33" t="s">
+        <v>324</v>
+      </c>
+      <c r="C33" t="s">
+        <v>326</v>
+      </c>
+      <c r="E33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>305</v>
+      </c>
+      <c r="B34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>305</v>
+      </c>
+      <c r="B35" t="s">
+        <v>327</v>
+      </c>
+      <c r="C35" t="s">
+        <v>326</v>
+      </c>
+      <c r="E35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>305</v>
+      </c>
+      <c r="B36" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>